<commit_message>
update - spreadsheet w/ 41-60
</commit_message>
<xml_diff>
--- a/scripts/evaluationStats.xlsx
+++ b/scripts/evaluationStats.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anasofiaribeiro/Desktop/Thesis/Refactor4Green/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28BB176-4FEE-1C41-817E-5215AB7E089B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F5637E-A603-8A47-8465-6E78BC7329B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apps" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>APPLICATION NAME</t>
   </si>
@@ -287,6 +297,132 @@
   </si>
   <si>
     <t>https://github.com/benjaminaigner/aiproute</t>
+  </si>
+  <si>
+    <t>Catfriend1/syncthing-android-fdroid</t>
+  </si>
+  <si>
+    <t>https://github.com/Catfriend1/syncthing-android-fdroid</t>
+  </si>
+  <si>
+    <t>hoihei/Silectric</t>
+  </si>
+  <si>
+    <t>https://github.com/hoihei/Silectric</t>
+  </si>
+  <si>
+    <t>arnowelzel/periodical</t>
+  </si>
+  <si>
+    <t>https://github.com/arnowelzel/periodical</t>
+  </si>
+  <si>
+    <t>ajh3/NoSurfForReddit</t>
+  </si>
+  <si>
+    <t>https://github.com/ajh3/NoSurfForReddit</t>
+  </si>
+  <si>
+    <t>fistons/TinyTinyFeed</t>
+  </si>
+  <si>
+    <t>https://github.com/fistons/TinyTinyFeed</t>
+  </si>
+  <si>
+    <t>Tortel/SysLog</t>
+  </si>
+  <si>
+    <t>https://github.com/Tortel/SysLog</t>
+  </si>
+  <si>
+    <t>mcastillof/FakeTraveler</t>
+  </si>
+  <si>
+    <t>https://github.com/mcastillof/FakeTraveler</t>
+  </si>
+  <si>
+    <t>apcro/leafpicrevived</t>
+  </si>
+  <si>
+    <t>https://github.com/apcro/leafpicrevived</t>
+  </si>
+  <si>
+    <t>fei0316/snapstreak-alarm</t>
+  </si>
+  <si>
+    <t>https://github.com/fei0316/snapstreak-alarm</t>
+  </si>
+  <si>
+    <t>devgianlu/DNSHero</t>
+  </si>
+  <si>
+    <t>https://github.com/devgianlu/DNSHero</t>
+  </si>
+  <si>
+    <t>js-labs/WalkieTalkie</t>
+  </si>
+  <si>
+    <t>https://github.com/js-labs/WalkieTalkie</t>
+  </si>
+  <si>
+    <t>TachibanaGeneralLaboratories/download-navi</t>
+  </si>
+  <si>
+    <t>https://github.com/TachibanaGeneralLaboratories/download-navi</t>
+  </si>
+  <si>
+    <t>k3b/LosslessJpgCrop</t>
+  </si>
+  <si>
+    <t>https://github.com/k3b/LosslessJpgCrop</t>
+  </si>
+  <si>
+    <t>nvllsvm/Audinaut</t>
+  </si>
+  <si>
+    <t>https://github.com/nvllsvm/Audinaut</t>
+  </si>
+  <si>
+    <t>tobykurien/BatteryFu</t>
+  </si>
+  <si>
+    <t>https://github.com/tobykurien/BatteryFu</t>
+  </si>
+  <si>
+    <t>bradand/XMouse</t>
+  </si>
+  <si>
+    <t>https://github.com/bradand/XMouse</t>
+  </si>
+  <si>
+    <t>knirirr/BeeCount</t>
+  </si>
+  <si>
+    <t>https://github.com/knirirr/BeeCount</t>
+  </si>
+  <si>
+    <t>SecUSo/privacy-friendly-pain-diary</t>
+  </si>
+  <si>
+    <t>https://github.com/SecUSo/privacy-friendly-pain-diary</t>
+  </si>
+  <si>
+    <t>btcontract/lnwallet</t>
+  </si>
+  <si>
+    <t>https://github.com/btcontract/lnwallet</t>
+  </si>
+  <si>
+    <t>devgianlu/PretendYoureXyzzyAndroid</t>
+  </si>
+  <si>
+    <t>https://github.com/devgianlu/PretendYoureXyzzyAndroid</t>
+  </si>
+  <si>
+    <t>Rudloff/lineageos-updater-shortcut</t>
+  </si>
+  <si>
+    <t>https://github.com/Rudloff/lineageos-updater-shortcut</t>
   </si>
 </sst>
 </file>
@@ -333,9 +469,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -679,13 +819,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1424,10 +1568,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>129</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1459,10 +1603,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1477,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1486,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1494,10 +1638,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1521,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1529,10 +1673,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1556,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1564,10 +1708,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1591,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1599,10 +1743,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1634,10 +1778,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1661,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1669,10 +1813,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1704,10 +1848,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1716,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1725,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -1739,10 +1883,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1751,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1760,13 +1904,13 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1774,10 +1918,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1809,10 +1953,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1844,10 +1988,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1868,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -1879,10 +2023,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1900,13 +2044,13 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1914,10 +2058,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1935,13 +2079,13 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -1949,10 +2093,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1984,10 +2128,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2019,10 +2163,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2043,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2054,36 +2198,771 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>87</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>88</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
         <v>0</v>
       </c>
     </row>
@@ -2109,8 +2988,14 @@
     <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B22" r:id="rId21" xr:uid="{1E1C86BB-519B-6D47-A71B-385747A7013E}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{C74821F6-38B4-FC4A-BB74-67A167B3D5A9}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{5338B409-5D5E-C243-B546-A005EF64F723}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{4AC2B82F-9353-B747-BBBF-741842066405}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{18B81C81-A2D4-7843-B555-C5FEBAA13887}"/>
+    <hyperlink ref="B42" r:id="rId24" xr:uid="{35A8D3AE-8920-E342-8EFA-1469D9A7CE2F}"/>
+    <hyperlink ref="B46" r:id="rId25" xr:uid="{56A3CB28-DE2D-564E-88EC-71E04CD587B9}"/>
+    <hyperlink ref="B53" r:id="rId26" xr:uid="{0E58EA01-E61A-3A4A-9DED-E6441FDAE6A9}"/>
+    <hyperlink ref="B60" r:id="rId27" xr:uid="{EC988BDD-A96A-B84B-A770-5F5D2798D44C}"/>
+    <hyperlink ref="B55" r:id="rId28" xr:uid="{4B0A2D53-7A90-A147-8832-3946A83D2565}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
decription + vender updates + action removed
</commit_message>
<xml_diff>
--- a/scripts/evaluationStats.xlsx
+++ b/scripts/evaluationStats.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anasofiaribeiro/Desktop/Thesis/Refactor4Green/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anasofiaribeiro/Desktop/Thesis/EcoAndroid/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DD4335-F4DC-1F45-B425-6044CAEE87E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDA924C-4173-E443-8D06-7D10B3339E0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apps" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="230">
   <si>
     <t>APPLICATION NAME</t>
   </si>
@@ -706,6 +707,21 @@
   </si>
   <si>
     <t>2 retirados</t>
+  </si>
+  <si>
+    <t>1 retirado</t>
+  </si>
+  <si>
+    <t>2 possible switch</t>
+  </si>
+  <si>
+    <t>1 retirado de CheckMetadata</t>
+  </si>
+  <si>
+    <t>CheckNetwork errr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 possible switch + 2 com clear intent </t>
   </si>
 </sst>
 </file>
@@ -728,12 +744,42 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -752,7 +798,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -763,12 +809,27 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1105,7 +1166,7 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1113,7 +1174,8 @@
     <col min="1" max="1" width="37.1640625" customWidth="1"/>
     <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -1154,54 +1216,57 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <f xml:space="preserve"> COUNTIFS(Q2:Q101, 10)</f>
-        <v>64</v>
-      </c>
-      <c r="P2">
-        <f t="shared" ref="P2:P33" si="0" xml:space="preserve"> COUNTIFS(C2:K2, 0)</f>
-        <v>6</v>
-      </c>
-      <c r="Q2">
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O2" s="5">
+        <f xml:space="preserve"> COUNTIFS(Q2:Q101, "&lt;10")</f>
+        <v>35</v>
+      </c>
+      <c r="P2" s="5">
+        <f xml:space="preserve"> COUNTIFS(C2:K2, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="Q2" s="5">
         <f xml:space="preserve"> COUNTIFS(C2:L2, 0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1243,10 +1308,10 @@
       </c>
       <c r="O3">
         <f xml:space="preserve"> 100 - O2</f>
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> COUNTIFS(C3:K3, 0)</f>
         <v>9</v>
       </c>
       <c r="Q3">
@@ -1254,48 +1319,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:P33" si="0" xml:space="preserve"> COUNTIFS(C4:K4, 0)</f>
         <v>8</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <f t="shared" ref="Q4:Q66" si="1" xml:space="preserve"> COUNTIFS(C4:L4, 0)</f>
         <v>9</v>
       </c>
@@ -1611,7 +1676,10 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>225</v>
       </c>
       <c r="P11">
         <f t="shared" si="0"/>
@@ -2006,7 +2074,7 @@
       </c>
       <c r="O19">
         <f>SUM(E2:E101)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P19">
         <f t="shared" si="0"/>
@@ -2112,7 +2180,7 @@
       </c>
       <c r="O21">
         <f>SUM(G2:G101)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="P21">
         <f t="shared" si="0"/>
@@ -2158,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" t="s">
         <v>216</v>
@@ -2173,7 +2241,7 @@
       </c>
       <c r="Q22">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -2218,7 +2286,7 @@
       </c>
       <c r="O23">
         <f>SUM(I2:I101)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P23">
         <f t="shared" si="0"/>
@@ -2377,7 +2445,7 @@
       </c>
       <c r="O26">
         <f xml:space="preserve">  SUM(L2:L101)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="P26">
         <f t="shared" si="0"/>
@@ -2425,6 +2493,10 @@
       <c r="L27">
         <v>0</v>
       </c>
+      <c r="O27">
+        <f xml:space="preserve"> SUM(O17:O26)</f>
+        <v>95</v>
+      </c>
       <c r="P27">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2530,7 +2602,7 @@
       <c r="A30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C30">
@@ -2723,7 +2795,7 @@
       </c>
       <c r="O33">
         <f>100 - COUNTIFS(E2:E101,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P33">
         <f t="shared" si="0"/>
@@ -2828,8 +2900,8 @@
         <v>215</v>
       </c>
       <c r="O35">
-        <f>100 - COUNTIFS(F1:F101,0)</f>
-        <v>0</v>
+        <f>100 - COUNTIFS(G2:G101,0)</f>
+        <v>6</v>
       </c>
       <c r="P35">
         <f t="shared" si="2"/>
@@ -3094,7 +3166,7 @@
       </c>
       <c r="O40">
         <f>100 - COUNTIFS(L2:L101,0)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="P40">
         <f t="shared" si="2"/>
@@ -3815,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3832,13 +3904,16 @@
       <c r="L56">
         <v>1</v>
       </c>
+      <c r="M56" t="s">
+        <v>227</v>
+      </c>
       <c r="P56">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q56">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
@@ -4014,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="L60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P60">
         <f t="shared" si="2"/>
@@ -4022,7 +4097,7 @@
       </c>
       <c r="Q60">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -4198,7 +4273,10 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M64" t="s">
+        <v>225</v>
       </c>
       <c r="P64">
         <f t="shared" si="2"/>
@@ -4229,7 +4307,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -4248,11 +4326,11 @@
       </c>
       <c r="P65">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q65">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
@@ -4419,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -4429,6 +4507,9 @@
       </c>
       <c r="L69">
         <v>0</v>
+      </c>
+      <c r="M69" t="s">
+        <v>229</v>
       </c>
       <c r="P69">
         <f t="shared" si="3"/>
@@ -4936,6 +5017,9 @@
       <c r="L80">
         <v>1</v>
       </c>
+      <c r="M80" t="s">
+        <v>226</v>
+      </c>
       <c r="P80">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -5302,7 +5386,7 @@
         <v>0</v>
       </c>
       <c r="L88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P88">
         <f t="shared" si="3"/>
@@ -5310,7 +5394,7 @@
       </c>
       <c r="Q88">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -5912,6 +5996,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -5946,7 +6035,343 @@
     <hyperlink ref="B94" r:id="rId31" xr:uid="{D022DEFE-707B-3B49-9F78-C5F8829F9FE8}"/>
     <hyperlink ref="B88" r:id="rId32" xr:uid="{D97E41EF-050E-5840-88D7-90C170781DB8}"/>
     <hyperlink ref="B65" r:id="rId33" xr:uid="{17445096-E7BF-5141-AACD-FD0E42666A31}"/>
+    <hyperlink ref="B30" r:id="rId34" xr:uid="{699A1B0D-4F57-294F-AB8F-88EA33001ADE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616ED232-1442-C846-8773-BBB76FCD26A0}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!D2:D101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!E2:E101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!F2:F101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!G2:G101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!H2:H101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> COUNTIFS(Apps!C2:C101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!E2:E101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!F2:F101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!G2:G101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!H2:H101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!D2:D101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!F2:F101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!G2:G101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!H2:H101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> COUNTIFS(Apps!E2:E101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101, "&gt;0", Apps!G2:G101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101, "&gt;0", Apps!H2:H101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101,  "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101,  "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101,  "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f xml:space="preserve"> COUNTIFS(Apps!F2:F101,  "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6">
+        <f xml:space="preserve"> COUNTIFS(Apps!G2:G101, "&gt;0", Apps!H2:H101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!G2:G101, "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!G2:G101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f xml:space="preserve"> COUNTIFS(Apps!G2:G101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <f xml:space="preserve"> COUNTIFS(Apps!G2:G101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7">
+        <f xml:space="preserve"> COUNTIFS(Apps!H2:H101, "&gt;0", Apps!I2:I101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <f xml:space="preserve"> COUNTIFS(Apps!H2:H101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> COUNTIFS(Apps!H2:H101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f xml:space="preserve"> COUNTIFS(Apps!H2:H101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="9">
+        <f xml:space="preserve"> COUNTIFS(Apps!I2:I101, "&gt;0", Apps!J2:J101, "&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> COUNTIFS(Apps!I2:I101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f xml:space="preserve"> COUNTIFS(Apps!K2:K101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9">
+        <f xml:space="preserve"> COUNTIFS(Apps!J2:J101, "&gt;0", Apps!K2:K101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <f xml:space="preserve"> COUNTIFS(Apps!J2:J101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10">
+        <f xml:space="preserve"> COUNTIFS(Apps!K2:K101, "&gt;0", Apps!L2:L101, "&gt;0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>